<commit_message>
Update on Skills to focus
</commit_message>
<xml_diff>
--- a/Documents/Perfomance Testing/PT TESTING.xlsx
+++ b/Documents/Perfomance Testing/PT TESTING.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Perfomance Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChandrasekarM\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A282588-EBAB-4BE9-9BA6-5D7C2B216F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E0B14A-9B97-4A15-9C19-B3585EBAFDD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{015BB451-B3AA-4A63-B2A7-78F6342B318D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{015BB451-B3AA-4A63-B2A7-78F6342B318D}"/>
   </bookViews>
   <sheets>
     <sheet name="General Concepts " sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="362">
   <si>
     <t>Controller</t>
   </si>
@@ -1086,6 +1086,45 @@
   </si>
   <si>
     <t>Understand Incident Management, Postmortems,Chaos ENgineering</t>
+  </si>
+  <si>
+    <t>AWR report,Thread Dump analsyis ,Heap Dump analysis</t>
+  </si>
+  <si>
+    <t>Performnce BottleNecks</t>
+  </si>
+  <si>
+    <t>App Dynamics</t>
+  </si>
+  <si>
+    <t>SAP protocol,Ajax truclient</t>
+  </si>
+  <si>
+    <t>Adobe analytics,Splunk</t>
+  </si>
+  <si>
+    <t>Jenkins</t>
+  </si>
+  <si>
+    <t>Master slave architeture/jmeter</t>
+  </si>
+  <si>
+    <t>Prometheus ,grafana,infllux</t>
+  </si>
+  <si>
+    <t>NeoLoad, Load Runner</t>
+  </si>
+  <si>
+    <t>K8S and Docker</t>
+  </si>
+  <si>
+    <t>git &amp; GitHub</t>
+  </si>
+  <si>
+    <t>Top Items to Focus</t>
+  </si>
+  <si>
+    <t>For 5 years Exp</t>
   </si>
 </sst>
 </file>
@@ -1159,9 +1198,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1199,7 +1238,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1305,7 +1344,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1447,7 +1486,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1461,18 +1500,18 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="72.5546875" customWidth="1"/>
+    <col min="1" max="1" width="72.54296875" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>214</v>
       </c>
@@ -1480,12 +1519,12 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -1493,7 +1532,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -1501,7 +1540,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>217</v>
       </c>
@@ -1509,7 +1548,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>218</v>
       </c>
@@ -1517,7 +1556,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>219</v>
       </c>
@@ -1525,7 +1564,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>220</v>
       </c>
@@ -1533,7 +1572,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>221</v>
       </c>
@@ -1541,7 +1580,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>222</v>
       </c>
@@ -1549,7 +1588,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>223</v>
       </c>
@@ -1557,7 +1596,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>224</v>
       </c>
@@ -1565,7 +1604,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>225</v>
       </c>
@@ -1573,7 +1612,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>226</v>
       </c>
@@ -1581,7 +1620,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>227</v>
       </c>
@@ -1589,7 +1628,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>228</v>
       </c>
@@ -1597,7 +1636,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>229</v>
       </c>
@@ -1605,7 +1644,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>230</v>
       </c>
@@ -1613,7 +1652,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>231</v>
       </c>
@@ -1621,7 +1660,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>232</v>
       </c>
@@ -1629,7 +1668,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>233</v>
       </c>
@@ -1637,7 +1676,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>234</v>
       </c>
@@ -1645,7 +1684,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>235</v>
       </c>
@@ -1653,7 +1692,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>236</v>
       </c>
@@ -1661,47 +1700,47 @@
         <v>305</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>314</v>
       </c>
@@ -1719,13 +1758,13 @@
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="80.6640625" customWidth="1"/>
-    <col min="2" max="2" width="65.77734375" customWidth="1"/>
+    <col min="1" max="1" width="80.6328125" customWidth="1"/>
+    <col min="2" max="2" width="65.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>131</v>
       </c>
@@ -1733,7 +1772,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -1741,7 +1780,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>132</v>
       </c>
@@ -1749,7 +1788,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>133</v>
       </c>
@@ -1757,7 +1796,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>134</v>
       </c>
@@ -1765,7 +1804,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -1773,7 +1812,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -1781,7 +1820,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -1789,7 +1828,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -1797,7 +1836,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>68</v>
       </c>
@@ -1805,7 +1844,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -1813,7 +1852,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -1821,7 +1860,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>135</v>
       </c>
@@ -1829,7 +1868,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -1837,7 +1876,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -1845,7 +1884,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -1853,7 +1892,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -1861,7 +1900,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -1869,7 +1908,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -1877,7 +1916,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>78</v>
       </c>
@@ -1885,7 +1924,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -1893,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -1901,7 +1940,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -1909,7 +1948,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -1917,7 +1956,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -1925,7 +1964,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>156</v>
       </c>
@@ -1933,7 +1972,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>157</v>
       </c>
@@ -1941,7 +1980,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>158</v>
       </c>
@@ -1949,7 +1988,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>159</v>
       </c>
@@ -1957,7 +1996,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>160</v>
       </c>
@@ -1965,7 +2004,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>161</v>
       </c>
@@ -1973,7 +2012,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>162</v>
       </c>
@@ -1981,7 +2020,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>163</v>
       </c>
@@ -1989,7 +2028,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>164</v>
       </c>
@@ -1997,7 +2036,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>165</v>
       </c>
@@ -2005,7 +2044,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>166</v>
       </c>
@@ -2013,7 +2052,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>167</v>
       </c>
@@ -2021,7 +2060,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>281</v>
       </c>
@@ -2029,67 +2068,67 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B42" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B49" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B53" s="1" t="s">
         <v>276</v>
       </c>
@@ -2107,13 +2146,13 @@
       <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="69.77734375" customWidth="1"/>
-    <col min="2" max="2" width="59.44140625" customWidth="1"/>
+    <col min="1" max="1" width="69.81640625" customWidth="1"/>
+    <col min="2" max="2" width="59.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
@@ -2121,7 +2160,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -2129,7 +2168,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -2137,7 +2176,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -2145,7 +2184,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -2153,7 +2192,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -2161,7 +2200,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -2169,7 +2208,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -2177,7 +2216,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -2185,7 +2224,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>68</v>
       </c>
@@ -2193,7 +2232,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -2201,7 +2240,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>70</v>
       </c>
@@ -2209,7 +2248,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>135</v>
       </c>
@@ -2217,7 +2256,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -2225,7 +2264,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -2233,7 +2272,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -2241,7 +2280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -2249,7 +2288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -2257,7 +2296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -2265,7 +2304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -2273,7 +2312,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -2281,7 +2320,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -2289,7 +2328,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -2297,7 +2336,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -2305,7 +2344,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -2313,7 +2352,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -2321,7 +2360,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>157</v>
       </c>
@@ -2329,7 +2368,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>158</v>
       </c>
@@ -2337,7 +2376,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>159</v>
       </c>
@@ -2345,7 +2384,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>160</v>
       </c>
@@ -2353,7 +2392,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>161</v>
       </c>
@@ -2361,7 +2400,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>182</v>
       </c>
@@ -2369,7 +2408,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>183</v>
       </c>
@@ -2377,7 +2416,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>184</v>
       </c>
@@ -2385,7 +2424,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>185</v>
       </c>
@@ -2393,7 +2432,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>186</v>
       </c>
@@ -2401,7 +2440,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>187</v>
       </c>
@@ -2409,7 +2448,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>188</v>
       </c>
@@ -2417,7 +2456,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>189</v>
       </c>
@@ -2425,7 +2464,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>190</v>
       </c>
@@ -2433,7 +2472,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>191</v>
       </c>
@@ -2441,7 +2480,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>192</v>
       </c>
@@ -2449,7 +2488,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>193</v>
       </c>
@@ -2457,7 +2496,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>84</v>
       </c>
@@ -2465,7 +2504,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -2473,7 +2512,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -2481,7 +2520,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>87</v>
       </c>
@@ -2489,7 +2528,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -2497,7 +2536,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>279</v>
       </c>
@@ -2505,7 +2544,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>89</v>
       </c>
@@ -2513,7 +2552,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>90</v>
       </c>
@@ -2521,7 +2560,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>91</v>
       </c>
@@ -2529,7 +2568,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>92</v>
       </c>
@@ -2537,7 +2576,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>93</v>
       </c>
@@ -2545,7 +2584,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>94</v>
       </c>
@@ -2553,7 +2592,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>280</v>
       </c>
@@ -2561,7 +2600,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>95</v>
       </c>
@@ -2569,7 +2608,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>96</v>
       </c>
@@ -2577,7 +2616,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>97</v>
       </c>
@@ -2585,7 +2624,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>98</v>
       </c>
@@ -2593,7 +2632,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>99</v>
       </c>
@@ -2601,7 +2640,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>100</v>
       </c>
@@ -2609,7 +2648,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>101</v>
       </c>
@@ -2617,7 +2656,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>102</v>
       </c>
@@ -2625,7 +2664,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>3</v>
       </c>
@@ -2633,7 +2672,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>103</v>
       </c>
@@ -2641,7 +2680,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>104</v>
       </c>
@@ -2649,7 +2688,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>105</v>
       </c>
@@ -2657,7 +2696,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>106</v>
       </c>
@@ -2665,7 +2704,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>107</v>
       </c>
@@ -2673,7 +2712,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>108</v>
       </c>
@@ -2681,7 +2720,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>109</v>
       </c>
@@ -2689,7 +2728,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>100</v>
       </c>
@@ -2697,7 +2736,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>194</v>
       </c>
@@ -2705,7 +2744,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>195</v>
       </c>
@@ -2713,7 +2752,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>196</v>
       </c>
@@ -2721,7 +2760,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>197</v>
       </c>
@@ -2729,7 +2768,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>198</v>
       </c>
@@ -2737,7 +2776,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>199</v>
       </c>
@@ -2745,7 +2784,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>200</v>
       </c>
@@ -2753,7 +2792,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>201</v>
       </c>
@@ -2761,7 +2800,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>202</v>
       </c>
@@ -2769,7 +2808,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>203</v>
       </c>
@@ -2777,7 +2816,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>204</v>
       </c>
@@ -2785,7 +2824,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>205</v>
       </c>
@@ -2793,7 +2832,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>206</v>
       </c>
@@ -2801,7 +2840,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>207</v>
       </c>
@@ -2809,7 +2848,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>208</v>
       </c>
@@ -2817,7 +2856,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>209</v>
       </c>
@@ -2825,7 +2864,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>210</v>
       </c>
@@ -2833,7 +2872,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>211</v>
       </c>
@@ -2841,22 +2880,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
         <v>56</v>
       </c>
@@ -2874,112 +2913,112 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="60.44140625" customWidth="1"/>
+    <col min="1" max="1" width="60.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>130</v>
       </c>
@@ -2997,12 +3036,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>327</v>
       </c>
@@ -3010,52 +3049,52 @@
         <v>316</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>326</v>
       </c>
@@ -3067,122 +3106,169 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DDC896C-F5ED-4B36-B21E-C1DB8CB6B2BD}">
-  <dimension ref="D3:E27"/>
+  <dimension ref="D1:N27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="4:14" x14ac:dyDescent="0.35">
+      <c r="J1" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="3" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D3" s="3" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="N3" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="4" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D4" s="2"/>
       <c r="E4" s="4" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="N4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="5" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D5" s="2"/>
       <c r="E5" s="4" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="N5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="6" spans="4:14" x14ac:dyDescent="0.35">
+      <c r="N6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="7" spans="4:14" x14ac:dyDescent="0.35">
       <c r="E7" s="4" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="N7" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="8" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D8" s="2"/>
       <c r="E8" s="4" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="N8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="9" spans="4:14" x14ac:dyDescent="0.35">
+      <c r="N9" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="10" spans="4:14" x14ac:dyDescent="0.35">
       <c r="E10" s="4" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="11" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="N10" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="11" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D11" s="2"/>
       <c r="E11" s="4" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="12" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="N11" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="12" spans="4:14" x14ac:dyDescent="0.35">
       <c r="E12" s="4" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="14" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="N12" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="13" spans="4:14" x14ac:dyDescent="0.35">
+      <c r="N13" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="14" spans="4:14" x14ac:dyDescent="0.35">
       <c r="D14" s="3" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="15" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="N14" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="15" spans="4:14" x14ac:dyDescent="0.35">
       <c r="E15" s="4" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="16" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:14" x14ac:dyDescent="0.35">
       <c r="E16" s="4" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E17" s="4" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E18" s="4" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E19" s="4" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D21" s="3" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E22" s="4" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E23" s="4" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E24" s="4" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E25" s="4" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E26" s="4" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E27" s="4" t="s">
         <v>348</v>
       </c>

</xml_diff>